<commit_message>
Finalizado até tarefa 5
</commit_message>
<xml_diff>
--- a/Modelagem/HROADS-Fisico.xlsx
+++ b/Modelagem/HROADS-Fisico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\desafio-HROADS\Modelagem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Desktop\SENAI\Desafio HROADS\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BF26DB-1371-49AF-AE53-B4B746203529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7320907A-0BC3-498A-8F29-DF73B8F80340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9EA8E97F-88A1-4632-BAAD-05E85D5AA331}"/>
+    <workbookView xWindow="-15360" yWindow="-2100" windowWidth="15375" windowHeight="7875" xr2:uid="{9EA8E97F-88A1-4632-BAAD-05E85D5AA331}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -329,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -451,6 +451,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,16 +771,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC46C1AD-5FA1-472E-8F62-8784FD703F7B}">
   <dimension ref="B2:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="13" width="21.81640625" customWidth="1"/>
+    <col min="2" max="13" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
@@ -789,7 +792,7 @@
       <c r="H2" s="36"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
@@ -813,7 +816,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <v>1</v>
       </c>
@@ -837,7 +840,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
         <v>2</v>
       </c>
@@ -861,7 +864,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="12">
         <v>3</v>
       </c>
@@ -885,7 +888,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -895,7 +898,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="37" t="s">
         <v>18</v>
       </c>
@@ -909,7 +912,7 @@
       <c r="H9" s="41"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>3</v>
       </c>
@@ -928,7 +931,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="15">
         <v>1</v>
       </c>
@@ -947,7 +950,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="15">
         <v>2</v>
       </c>
@@ -966,7 +969,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="15">
         <v>3</v>
       </c>
@@ -985,7 +988,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="15">
         <v>4</v>
       </c>
@@ -1004,12 +1007,12 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="15">
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="2">
@@ -1023,14 +1026,13 @@
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="15">
         <v>6</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="1"/>
+      <c r="C16" s="42" t="s">
+        <v>31</v>
+      </c>
       <c r="F16" s="2">
         <v>6</v>
       </c>
@@ -1042,7 +1044,7 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <v>7</v>
       </c>
@@ -1065,7 +1067,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F18" s="2">
         <v>8</v>
       </c>
@@ -1076,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F19" s="2">
         <v>9</v>
       </c>
@@ -1087,12 +1089,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F20" s="5"/>
       <c r="G20" s="6"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="32" t="s">
         <v>1</v>
       </c>
@@ -1103,7 +1105,7 @@
       <c r="G22" s="30"/>
       <c r="H22" s="31"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
         <v>34</v>
       </c>
@@ -1121,7 +1123,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="19">
         <v>1</v>
       </c>
@@ -1139,7 +1141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="19">
         <v>2</v>
       </c>
@@ -1157,7 +1159,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="19">
         <v>3</v>
       </c>
@@ -1175,7 +1177,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="21">
         <v>4</v>
       </c>
@@ -1184,38 +1186,38 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -1230,5 +1232,6 @@
     <mergeCell ref="F9:H9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>